<commit_message>
more tests and improvements
</commit_message>
<xml_diff>
--- a/experiments.xlsx
+++ b/experiments.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="17830"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="17927"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
@@ -9,10 +9,11 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="21570" windowHeight="7965"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="21570" windowHeight="7965" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="agility" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="171027"/>
   <extLst>
@@ -24,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="90" uniqueCount="25">
   <si>
     <t>benchmark full</t>
   </si>
@@ -69,6 +70,36 @@
   </si>
   <si>
     <t>solve</t>
+  </si>
+  <si>
+    <t>BENCHMARK</t>
+  </si>
+  <si>
+    <t>SPEED</t>
+  </si>
+  <si>
+    <t>ACC</t>
+  </si>
+  <si>
+    <t>LOW</t>
+  </si>
+  <si>
+    <t>MED</t>
+  </si>
+  <si>
+    <t>HIGH</t>
+  </si>
+  <si>
+    <t>SF</t>
+  </si>
+  <si>
+    <t>-</t>
+  </si>
+  <si>
+    <t>LEUVEN</t>
+  </si>
+  <si>
+    <t>SCORES</t>
   </si>
 </sst>
 </file>
@@ -422,7 +453,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M42"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B21" workbookViewId="0">
+    <sheetView topLeftCell="B21" workbookViewId="0">
       <selection activeCell="S34" sqref="S34"/>
     </sheetView>
   </sheetViews>
@@ -945,4 +976,372 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:P15"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="O16" sqref="O16"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>15</v>
+      </c>
+      <c r="G1" t="s">
+        <v>21</v>
+      </c>
+      <c r="M1" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="2" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="B2" t="s">
+        <v>16</v>
+      </c>
+      <c r="H2" t="s">
+        <v>16</v>
+      </c>
+      <c r="N2" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="3" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>17</v>
+      </c>
+      <c r="B3" t="s">
+        <v>18</v>
+      </c>
+      <c r="C3" t="s">
+        <v>19</v>
+      </c>
+      <c r="D3" t="s">
+        <v>20</v>
+      </c>
+      <c r="G3" t="s">
+        <v>17</v>
+      </c>
+      <c r="H3" t="s">
+        <v>18</v>
+      </c>
+      <c r="I3" t="s">
+        <v>19</v>
+      </c>
+      <c r="J3" t="s">
+        <v>20</v>
+      </c>
+      <c r="M3" t="s">
+        <v>17</v>
+      </c>
+      <c r="N3" t="s">
+        <v>18</v>
+      </c>
+      <c r="O3" t="s">
+        <v>19</v>
+      </c>
+      <c r="P3" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="4" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>18</v>
+      </c>
+      <c r="B4">
+        <v>33.159999999999997</v>
+      </c>
+      <c r="C4">
+        <v>18.329999999999998</v>
+      </c>
+      <c r="D4">
+        <v>132.07</v>
+      </c>
+      <c r="G4" t="s">
+        <v>18</v>
+      </c>
+      <c r="H4">
+        <v>135.19</v>
+      </c>
+      <c r="I4">
+        <v>960.39</v>
+      </c>
+      <c r="J4" t="s">
+        <v>22</v>
+      </c>
+      <c r="M4" t="s">
+        <v>18</v>
+      </c>
+      <c r="N4">
+        <v>402.68</v>
+      </c>
+      <c r="O4" t="s">
+        <v>22</v>
+      </c>
+      <c r="P4" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="5" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>19</v>
+      </c>
+      <c r="B5">
+        <v>8.91</v>
+      </c>
+      <c r="C5">
+        <v>17.2</v>
+      </c>
+      <c r="D5">
+        <v>34.700000000000003</v>
+      </c>
+      <c r="G5" t="s">
+        <v>19</v>
+      </c>
+      <c r="H5">
+        <v>37.74</v>
+      </c>
+      <c r="I5">
+        <v>65.84</v>
+      </c>
+      <c r="J5">
+        <v>800.51</v>
+      </c>
+      <c r="M5" t="s">
+        <v>19</v>
+      </c>
+      <c r="N5">
+        <v>139.88999999999999</v>
+      </c>
+      <c r="O5">
+        <v>311.73</v>
+      </c>
+      <c r="P5" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="6" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>20</v>
+      </c>
+      <c r="B6">
+        <v>7.35</v>
+      </c>
+      <c r="C6">
+        <v>5.65</v>
+      </c>
+      <c r="D6">
+        <v>4.82</v>
+      </c>
+      <c r="G6" t="s">
+        <v>20</v>
+      </c>
+      <c r="H6">
+        <v>25.9</v>
+      </c>
+      <c r="I6">
+        <v>22.24</v>
+      </c>
+      <c r="J6">
+        <v>93.68</v>
+      </c>
+      <c r="M6" t="s">
+        <v>20</v>
+      </c>
+      <c r="N6">
+        <v>99.5</v>
+      </c>
+      <c r="O6">
+        <v>119.17</v>
+      </c>
+      <c r="P6" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="9" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="10" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>15</v>
+      </c>
+      <c r="G10" t="s">
+        <v>21</v>
+      </c>
+      <c r="M10" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="11" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="B11" t="s">
+        <v>16</v>
+      </c>
+      <c r="H11" t="s">
+        <v>16</v>
+      </c>
+      <c r="N11" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="12" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>17</v>
+      </c>
+      <c r="B12" t="s">
+        <v>18</v>
+      </c>
+      <c r="C12" t="s">
+        <v>19</v>
+      </c>
+      <c r="D12" t="s">
+        <v>20</v>
+      </c>
+      <c r="G12" t="s">
+        <v>17</v>
+      </c>
+      <c r="H12" t="s">
+        <v>18</v>
+      </c>
+      <c r="I12" t="s">
+        <v>19</v>
+      </c>
+      <c r="J12" t="s">
+        <v>20</v>
+      </c>
+      <c r="M12" t="s">
+        <v>17</v>
+      </c>
+      <c r="N12" t="s">
+        <v>18</v>
+      </c>
+      <c r="O12" t="s">
+        <v>19</v>
+      </c>
+      <c r="P12" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="13" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>18</v>
+      </c>
+      <c r="B13">
+        <v>98.88</v>
+      </c>
+      <c r="C13">
+        <v>84.96</v>
+      </c>
+      <c r="D13">
+        <v>83.52</v>
+      </c>
+      <c r="G13" t="s">
+        <v>18</v>
+      </c>
+      <c r="H13">
+        <v>305.45</v>
+      </c>
+      <c r="I13">
+        <v>150.13</v>
+      </c>
+      <c r="J13" t="s">
+        <v>22</v>
+      </c>
+      <c r="M13" t="s">
+        <v>18</v>
+      </c>
+      <c r="N13">
+        <v>280.92</v>
+      </c>
+      <c r="O13" t="s">
+        <v>22</v>
+      </c>
+      <c r="P13" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="14" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>19</v>
+      </c>
+      <c r="B14">
+        <v>93.4</v>
+      </c>
+      <c r="C14">
+        <v>45.12</v>
+      </c>
+      <c r="D14">
+        <v>47.4</v>
+      </c>
+      <c r="G14" t="s">
+        <v>19</v>
+      </c>
+      <c r="H14">
+        <v>317.32</v>
+      </c>
+      <c r="I14">
+        <v>107.72</v>
+      </c>
+      <c r="J14">
+        <v>74.2</v>
+      </c>
+      <c r="M14" t="s">
+        <v>19</v>
+      </c>
+      <c r="N14">
+        <v>284.39999999999998</v>
+      </c>
+      <c r="O14">
+        <v>99.6</v>
+      </c>
+      <c r="P14" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="15" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>20</v>
+      </c>
+      <c r="B15">
+        <v>96</v>
+      </c>
+      <c r="C15">
+        <v>48.44</v>
+      </c>
+      <c r="D15">
+        <v>33.15</v>
+      </c>
+      <c r="G15" t="s">
+        <v>20</v>
+      </c>
+      <c r="H15">
+        <v>321.10000000000002</v>
+      </c>
+      <c r="I15">
+        <v>108.52</v>
+      </c>
+      <c r="J15">
+        <v>61.8</v>
+      </c>
+      <c r="M15" t="s">
+        <v>20</v>
+      </c>
+      <c r="N15">
+        <v>295.7</v>
+      </c>
+      <c r="O15">
+        <v>101.73</v>
+      </c>
+      <c r="P15" t="s">
+        <v>22</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
discussion and conclusion nearly complete
</commit_message>
<xml_diff>
--- a/experiments.xlsx
+++ b/experiments.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="21570" windowHeight="7965" tabRatio="682" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="21570" windowHeight="7965" tabRatio="682" activeTab="5"/>
   </bookViews>
   <sheets>
     <sheet name="convexity" sheetId="7" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="208" uniqueCount="75">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="212" uniqueCount="79">
   <si>
     <t>BENCHMARK</t>
   </si>
@@ -258,6 +258,18 @@
   </si>
   <si>
     <t>length/seg</t>
+  </si>
+  <si>
+    <t>edges</t>
+  </si>
+  <si>
+    <t>edge/obs</t>
+  </si>
+  <si>
+    <t>time std ratio</t>
+  </si>
+  <si>
+    <t>score std  ratio</t>
   </si>
 </sst>
 </file>
@@ -5440,7 +5452,7 @@
             </a:r>
             <a:r>
               <a:rPr lang="nl-BE" baseline="0"/>
-              <a:t> vertices</a:t>
+              <a:t> edges</a:t>
             </a:r>
             <a:endParaRPr lang="nl-BE"/>
           </a:p>
@@ -5682,31 +5694,31 @@
                 <c:ptCount val="9"/>
                 <c:lvl>
                   <c:pt idx="0">
-                    <c:v>6</c:v>
+                    <c:v>20</c:v>
                   </c:pt>
                   <c:pt idx="1">
-                    <c:v>12</c:v>
+                    <c:v>40</c:v>
                   </c:pt>
                   <c:pt idx="2">
-                    <c:v>24</c:v>
+                    <c:v>80</c:v>
                   </c:pt>
                   <c:pt idx="3">
-                    <c:v>6</c:v>
+                    <c:v>20</c:v>
                   </c:pt>
                   <c:pt idx="4">
-                    <c:v>12</c:v>
+                    <c:v>40</c:v>
                   </c:pt>
                   <c:pt idx="5">
-                    <c:v>24</c:v>
+                    <c:v>80</c:v>
                   </c:pt>
                   <c:pt idx="6">
-                    <c:v>6</c:v>
+                    <c:v>20</c:v>
                   </c:pt>
                   <c:pt idx="7">
-                    <c:v>12</c:v>
+                    <c:v>40</c:v>
                   </c:pt>
                   <c:pt idx="8">
-                    <c:v>24</c:v>
+                    <c:v>80</c:v>
                   </c:pt>
                 </c:lvl>
                 <c:lvl>
@@ -5972,31 +5984,31 @@
                 <c:ptCount val="9"/>
                 <c:lvl>
                   <c:pt idx="0">
-                    <c:v>6</c:v>
+                    <c:v>20</c:v>
                   </c:pt>
                   <c:pt idx="1">
-                    <c:v>12</c:v>
+                    <c:v>40</c:v>
                   </c:pt>
                   <c:pt idx="2">
-                    <c:v>24</c:v>
+                    <c:v>80</c:v>
                   </c:pt>
                   <c:pt idx="3">
-                    <c:v>6</c:v>
+                    <c:v>20</c:v>
                   </c:pt>
                   <c:pt idx="4">
-                    <c:v>12</c:v>
+                    <c:v>40</c:v>
                   </c:pt>
                   <c:pt idx="5">
-                    <c:v>24</c:v>
+                    <c:v>80</c:v>
                   </c:pt>
                   <c:pt idx="6">
-                    <c:v>6</c:v>
+                    <c:v>20</c:v>
                   </c:pt>
                   <c:pt idx="7">
-                    <c:v>12</c:v>
+                    <c:v>40</c:v>
                   </c:pt>
                   <c:pt idx="8">
-                    <c:v>24</c:v>
+                    <c:v>80</c:v>
                   </c:pt>
                 </c:lvl>
                 <c:lvl>
@@ -6217,31 +6229,31 @@
                       <c:ptCount val="9"/>
                       <c:lvl>
                         <c:pt idx="0">
-                          <c:v>6</c:v>
+                          <c:v>20</c:v>
                         </c:pt>
                         <c:pt idx="1">
-                          <c:v>12</c:v>
+                          <c:v>40</c:v>
                         </c:pt>
                         <c:pt idx="2">
-                          <c:v>24</c:v>
+                          <c:v>80</c:v>
                         </c:pt>
                         <c:pt idx="3">
-                          <c:v>6</c:v>
+                          <c:v>20</c:v>
                         </c:pt>
                         <c:pt idx="4">
-                          <c:v>12</c:v>
+                          <c:v>40</c:v>
                         </c:pt>
                         <c:pt idx="5">
-                          <c:v>24</c:v>
+                          <c:v>80</c:v>
                         </c:pt>
                         <c:pt idx="6">
-                          <c:v>6</c:v>
+                          <c:v>20</c:v>
                         </c:pt>
                         <c:pt idx="7">
-                          <c:v>12</c:v>
+                          <c:v>40</c:v>
                         </c:pt>
                         <c:pt idx="8">
-                          <c:v>24</c:v>
+                          <c:v>80</c:v>
                         </c:pt>
                       </c:lvl>
                       <c:lvl>
@@ -6415,31 +6427,31 @@
                       <c:ptCount val="9"/>
                       <c:lvl>
                         <c:pt idx="0">
-                          <c:v>6</c:v>
+                          <c:v>20</c:v>
                         </c:pt>
                         <c:pt idx="1">
-                          <c:v>12</c:v>
+                          <c:v>40</c:v>
                         </c:pt>
                         <c:pt idx="2">
-                          <c:v>24</c:v>
+                          <c:v>80</c:v>
                         </c:pt>
                         <c:pt idx="3">
-                          <c:v>6</c:v>
+                          <c:v>20</c:v>
                         </c:pt>
                         <c:pt idx="4">
-                          <c:v>12</c:v>
+                          <c:v>40</c:v>
                         </c:pt>
                         <c:pt idx="5">
-                          <c:v>24</c:v>
+                          <c:v>80</c:v>
                         </c:pt>
                         <c:pt idx="6">
-                          <c:v>6</c:v>
+                          <c:v>20</c:v>
                         </c:pt>
                         <c:pt idx="7">
-                          <c:v>12</c:v>
+                          <c:v>40</c:v>
                         </c:pt>
                         <c:pt idx="8">
-                          <c:v>24</c:v>
+                          <c:v>80</c:v>
                         </c:pt>
                       </c:lvl>
                       <c:lvl>
@@ -7013,6 +7025,39 @@
           </c:spPr>
           <c:invertIfNegative val="0"/>
           <c:dLbls>
+            <c:dLbl>
+              <c:idx val="2"/>
+              <c:tx>
+                <c:rich>
+                  <a:bodyPr/>
+                  <a:lstStyle/>
+                  <a:p>
+                    <a:fld id="{82C1F054-3B55-4F8E-BCA4-952E2AFFD793}" type="VALUE">
+                      <a:rPr lang="en-US"/>
+                      <a:pPr/>
+                      <a:t>[VALUE]</a:t>
+                    </a:fld>
+                    <a:endParaRPr lang="nl-BE"/>
+                  </a:p>
+                </c:rich>
+              </c:tx>
+              <c:dLblPos val="inBase"/>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="1"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:showBubbleSize val="0"/>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                  <c15:dlblFieldTable/>
+                  <c15:showDataLabelsRange val="0"/>
+                </c:ext>
+                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                  <c16:uniqueId val="{00000000-8A9A-4484-82F2-4A65FCB8604D}"/>
+                </c:ext>
+              </c:extLst>
+            </c:dLbl>
             <c:spPr>
               <a:noFill/>
               <a:ln>
@@ -11784,7 +11829,7 @@
           <c:order val="9"/>
           <c:tx>
             <c:strRef>
-              <c:f>general!$A$11</c:f>
+              <c:f>general!$A$13</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -11842,7 +11887,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>general!$B$11:$J$11</c:f>
+              <c:f>general!$B$13:$J$13</c:f>
               <c:numCache>
                 <c:formatCode>0.00</c:formatCode>
                 <c:ptCount val="9"/>
@@ -11887,7 +11932,7 @@
           <c:order val="10"/>
           <c:tx>
             <c:strRef>
-              <c:f>general!$A$12</c:f>
+              <c:f>general!$A$14</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -11945,7 +11990,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>general!$B$12:$J$12</c:f>
+              <c:f>general!$B$14:$J$14</c:f>
               <c:numCache>
                 <c:formatCode>0.00</c:formatCode>
                 <c:ptCount val="9"/>
@@ -11990,7 +12035,7 @@
           <c:order val="11"/>
           <c:tx>
             <c:strRef>
-              <c:f>general!$A$13</c:f>
+              <c:f>general!$A$15</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -12048,7 +12093,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>general!$B$13:$J$13</c:f>
+              <c:f>general!$B$15:$J$15</c:f>
               <c:numCache>
                 <c:formatCode>0.00</c:formatCode>
                 <c:ptCount val="9"/>
@@ -12093,7 +12138,7 @@
           <c:order val="12"/>
           <c:tx>
             <c:strRef>
-              <c:f>general!$A$14</c:f>
+              <c:f>general!$A$16</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -12152,7 +12197,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>general!$B$14:$J$14</c:f>
+              <c:f>general!$B$16:$J$16</c:f>
               <c:numCache>
                 <c:formatCode>0.00</c:formatCode>
                 <c:ptCount val="9"/>
@@ -12300,10 +12345,10 @@
                         <c:v>11</c:v>
                       </c:pt>
                       <c:pt idx="3">
-                        <c:v>684</c:v>
+                        <c:v>1235</c:v>
                       </c:pt>
                       <c:pt idx="4">
-                        <c:v>684</c:v>
+                        <c:v>1235</c:v>
                       </c:pt>
                       <c:pt idx="5">
                         <c:v>6580</c:v>
@@ -12336,7 +12381,7 @@
                     <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                       <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                         <c15:formulaRef>
-                          <c15:sqref>general!$A$3</c15:sqref>
+                          <c15:sqref>general!$A$5</c15:sqref>
                         </c15:formulaRef>
                       </c:ext>
                     </c:extLst>
@@ -12404,7 +12449,7 @@
                     <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                       <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                         <c15:formulaRef>
-                          <c15:sqref>general!$B$3:$J$3</c15:sqref>
+                          <c15:sqref>general!$B$5:$J$5</c15:sqref>
                         </c15:formulaRef>
                       </c:ext>
                     </c:extLst>
@@ -12457,7 +12502,7 @@
                     <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                       <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                         <c15:formulaRef>
-                          <c15:sqref>general!$A$4</c15:sqref>
+                          <c15:sqref>general!$A$6</c15:sqref>
                         </c15:formulaRef>
                       </c:ext>
                     </c:extLst>
@@ -12525,7 +12570,7 @@
                     <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                       <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                         <c15:formulaRef>
-                          <c15:sqref>general!$B$4:$J$4</c15:sqref>
+                          <c15:sqref>general!$B$6:$J$6</c15:sqref>
                         </c15:formulaRef>
                       </c:ext>
                     </c:extLst>
@@ -12578,7 +12623,7 @@
                     <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                       <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                         <c15:formulaRef>
-                          <c15:sqref>general!$A$5</c15:sqref>
+                          <c15:sqref>general!$A$7</c15:sqref>
                         </c15:formulaRef>
                       </c:ext>
                     </c:extLst>
@@ -12646,7 +12691,7 @@
                     <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                       <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                         <c15:formulaRef>
-                          <c15:sqref>general!$B$5:$J$5</c15:sqref>
+                          <c15:sqref>general!$B$7:$J$7</c15:sqref>
                         </c15:formulaRef>
                       </c:ext>
                     </c:extLst>
@@ -12699,7 +12744,7 @@
                     <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                       <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                         <c15:formulaRef>
-                          <c15:sqref>general!$A$6</c15:sqref>
+                          <c15:sqref>general!$A$8</c15:sqref>
                         </c15:formulaRef>
                       </c:ext>
                     </c:extLst>
@@ -12767,7 +12812,7 @@
                     <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                       <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                         <c15:formulaRef>
-                          <c15:sqref>general!$B$6:$J$6</c15:sqref>
+                          <c15:sqref>general!$B$8:$J$8</c15:sqref>
                         </c15:formulaRef>
                       </c:ext>
                     </c:extLst>
@@ -12820,7 +12865,7 @@
                     <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                       <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                         <c15:formulaRef>
-                          <c15:sqref>general!$A$7</c15:sqref>
+                          <c15:sqref>general!$A$9</c15:sqref>
                         </c15:formulaRef>
                       </c:ext>
                     </c:extLst>
@@ -12888,7 +12933,7 @@
                     <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                       <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                         <c15:formulaRef>
-                          <c15:sqref>general!$B$7:$J$7</c15:sqref>
+                          <c15:sqref>general!$B$9:$J$9</c15:sqref>
                         </c15:formulaRef>
                       </c:ext>
                     </c:extLst>
@@ -12941,7 +12986,7 @@
                     <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                       <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                         <c15:formulaRef>
-                          <c15:sqref>general!$A$8</c15:sqref>
+                          <c15:sqref>general!$A$10</c15:sqref>
                         </c15:formulaRef>
                       </c:ext>
                     </c:extLst>
@@ -13011,7 +13056,7 @@
                     <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                       <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                         <c15:formulaRef>
-                          <c15:sqref>general!$B$8:$J$8</c15:sqref>
+                          <c15:sqref>general!$B$10:$J$10</c15:sqref>
                         </c15:formulaRef>
                       </c:ext>
                     </c:extLst>
@@ -13064,7 +13109,7 @@
                     <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                       <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                         <c15:formulaRef>
-                          <c15:sqref>general!$A$9</c15:sqref>
+                          <c15:sqref>general!$A$11</c15:sqref>
                         </c15:formulaRef>
                       </c:ext>
                     </c:extLst>
@@ -13134,7 +13179,7 @@
                     <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                       <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                         <c15:formulaRef>
-                          <c15:sqref>general!$B$9:$J$9</c15:sqref>
+                          <c15:sqref>general!$B$11:$J$11</c15:sqref>
                         </c15:formulaRef>
                       </c:ext>
                     </c:extLst>
@@ -13187,7 +13232,7 @@
                     <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                       <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                         <c15:formulaRef>
-                          <c15:sqref>general!$A$10</c15:sqref>
+                          <c15:sqref>general!$A$12</c15:sqref>
                         </c15:formulaRef>
                       </c:ext>
                     </c:extLst>
@@ -13257,7 +13302,7 @@
                     <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                       <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                         <c15:formulaRef>
-                          <c15:sqref>general!$B$10:$J$10</c15:sqref>
+                          <c15:sqref>general!$B$12:$J$12</c15:sqref>
                         </c15:formulaRef>
                       </c:ext>
                     </c:extLst>
@@ -13310,7 +13355,7 @@
                     <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                       <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                         <c15:formulaRef>
-                          <c15:sqref>general!$A$15</c15:sqref>
+                          <c15:sqref>general!$A$17</c15:sqref>
                         </c15:formulaRef>
                       </c:ext>
                     </c:extLst>
@@ -13381,7 +13426,7 @@
                     <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                       <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                         <c15:formulaRef>
-                          <c15:sqref>general!$B$15:$J$15</c15:sqref>
+                          <c15:sqref>general!$B$17:$J$17</c15:sqref>
                         </c15:formulaRef>
                       </c:ext>
                     </c:extLst>
@@ -27512,13 +27557,13 @@
     <xdr:from>
       <xdr:col>2</xdr:col>
       <xdr:colOff>838200</xdr:colOff>
-      <xdr:row>16</xdr:row>
+      <xdr:row>18</xdr:row>
       <xdr:rowOff>19050</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>8</xdr:col>
       <xdr:colOff>38100</xdr:colOff>
-      <xdr:row>30</xdr:row>
+      <xdr:row>32</xdr:row>
       <xdr:rowOff>95250</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
@@ -28983,10 +29028,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J15"/>
+  <dimension ref="A1:J17"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L10" sqref="L10"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="J2" sqref="J2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -29037,10 +29082,10 @@
         <v>11</v>
       </c>
       <c r="E2">
-        <v>684</v>
+        <v>1235</v>
       </c>
       <c r="F2">
-        <v>684</v>
+        <v>1235</v>
       </c>
       <c r="G2">
         <v>6580</v>
@@ -29057,462 +29102,535 @@
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>48</v>
-      </c>
-      <c r="B3" t="s">
-        <v>64</v>
-      </c>
-      <c r="C3" t="s">
-        <v>65</v>
-      </c>
-      <c r="D3" t="s">
-        <v>68</v>
-      </c>
-      <c r="E3" t="s">
-        <v>66</v>
-      </c>
-      <c r="F3" t="s">
-        <v>66</v>
-      </c>
-      <c r="G3" t="s">
-        <v>67</v>
-      </c>
-      <c r="H3" t="s">
-        <v>66</v>
-      </c>
-      <c r="I3" t="s">
-        <v>66</v>
-      </c>
-      <c r="J3" t="s">
-        <v>67</v>
+        <v>75</v>
+      </c>
+      <c r="B3">
+        <v>20</v>
+      </c>
+      <c r="C3">
+        <v>36</v>
+      </c>
+      <c r="D3">
+        <v>44</v>
+      </c>
+      <c r="E3">
+        <v>4940</v>
+      </c>
+      <c r="F3">
+        <v>4940</v>
+      </c>
+      <c r="G3">
+        <v>26320</v>
+      </c>
+      <c r="H3">
+        <v>19941</v>
+      </c>
+      <c r="I3">
+        <v>19941</v>
+      </c>
+      <c r="J3">
+        <v>111998</v>
       </c>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>49</v>
+        <v>76</v>
       </c>
       <c r="B4">
-        <v>88</v>
+        <f>B3/B2</f>
+        <v>4</v>
       </c>
       <c r="C4">
-        <v>146</v>
+        <f t="shared" ref="C4:J4" si="0">C3/C2</f>
+        <v>4</v>
       </c>
       <c r="D4">
-        <v>96</v>
+        <f t="shared" si="0"/>
+        <v>4</v>
       </c>
       <c r="E4">
-        <v>1392</v>
+        <f t="shared" si="0"/>
+        <v>4</v>
       </c>
       <c r="F4">
-        <v>1490</v>
+        <f t="shared" si="0"/>
+        <v>4</v>
       </c>
       <c r="G4">
-        <v>4325</v>
+        <f t="shared" si="0"/>
+        <v>4</v>
       </c>
       <c r="H4">
-        <v>1312</v>
+        <f t="shared" si="0"/>
+        <v>6.476453393959078</v>
       </c>
       <c r="I4">
-        <v>864</v>
+        <f t="shared" si="0"/>
+        <v>6.476453393959078</v>
       </c>
       <c r="J4">
-        <v>3041</v>
+        <f t="shared" si="0"/>
+        <v>5.9333545242636152</v>
       </c>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>50</v>
-      </c>
-      <c r="B5">
-        <v>7</v>
-      </c>
-      <c r="C5">
-        <v>11</v>
-      </c>
-      <c r="D5">
-        <v>10</v>
-      </c>
-      <c r="E5">
-        <v>34</v>
-      </c>
-      <c r="F5">
-        <v>38</v>
-      </c>
-      <c r="G5">
-        <v>107</v>
-      </c>
-      <c r="H5">
-        <v>34</v>
-      </c>
-      <c r="I5">
-        <v>22</v>
-      </c>
-      <c r="J5">
-        <v>78</v>
+        <v>48</v>
+      </c>
+      <c r="B5" t="s">
+        <v>64</v>
+      </c>
+      <c r="C5" t="s">
+        <v>65</v>
+      </c>
+      <c r="D5" t="s">
+        <v>68</v>
+      </c>
+      <c r="E5" t="s">
+        <v>66</v>
+      </c>
+      <c r="F5" t="s">
+        <v>66</v>
+      </c>
+      <c r="G5" t="s">
+        <v>67</v>
+      </c>
+      <c r="H5" t="s">
+        <v>66</v>
+      </c>
+      <c r="I5" t="s">
+        <v>66</v>
+      </c>
+      <c r="J5" t="s">
+        <v>67</v>
       </c>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="B6">
-        <v>0</v>
+        <v>88</v>
       </c>
       <c r="C6">
-        <v>0</v>
+        <v>146</v>
       </c>
       <c r="D6">
-        <v>0.01</v>
+        <v>96</v>
       </c>
       <c r="E6">
-        <v>1.37</v>
+        <v>1392</v>
       </c>
       <c r="F6">
-        <v>1.82</v>
+        <v>1490</v>
       </c>
       <c r="G6">
-        <v>15.88</v>
+        <v>4325</v>
       </c>
       <c r="H6">
-        <v>1.51</v>
+        <v>1312</v>
       </c>
       <c r="I6">
-        <v>0.53</v>
+        <v>864</v>
       </c>
       <c r="J6">
-        <v>14.65</v>
+        <v>3041</v>
       </c>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="B7">
-        <v>0.33</v>
+        <v>7</v>
       </c>
       <c r="C7">
-        <v>0.65</v>
+        <v>11</v>
       </c>
       <c r="D7">
-        <v>1.06</v>
+        <v>10</v>
       </c>
       <c r="E7">
-        <v>7.68</v>
+        <v>34</v>
       </c>
       <c r="F7">
-        <v>7.98</v>
+        <v>38</v>
       </c>
       <c r="G7">
-        <v>15.41</v>
+        <v>107</v>
       </c>
       <c r="H7">
-        <v>23.49</v>
+        <v>34</v>
       </c>
       <c r="I7">
-        <v>14</v>
+        <v>22</v>
       </c>
       <c r="J7">
-        <v>67.55</v>
+        <v>78</v>
       </c>
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="B8">
-        <v>10.48</v>
+        <v>0</v>
       </c>
       <c r="C8">
-        <v>17.95</v>
+        <v>0</v>
       </c>
       <c r="D8">
-        <v>7.17</v>
+        <v>0.01</v>
       </c>
       <c r="E8">
-        <v>32.81</v>
+        <v>1.37</v>
       </c>
       <c r="F8">
-        <v>36.81</v>
+        <v>1.82</v>
       </c>
       <c r="G8">
-        <v>75.44</v>
+        <v>15.88</v>
       </c>
       <c r="H8">
-        <v>135.86000000000001</v>
+        <v>1.51</v>
       </c>
       <c r="I8">
-        <v>62.03</v>
+        <v>0.53</v>
       </c>
       <c r="J8">
-        <v>460.46</v>
+        <v>14.65</v>
       </c>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>63</v>
+        <v>52</v>
       </c>
       <c r="B9">
-        <v>10.97</v>
+        <v>0.33</v>
       </c>
       <c r="C9">
-        <v>18.87</v>
+        <v>0.65</v>
       </c>
       <c r="D9">
-        <v>8.4600000000000009</v>
+        <v>1.06</v>
       </c>
       <c r="E9">
-        <v>42.43</v>
+        <v>7.68</v>
       </c>
       <c r="F9">
-        <v>47.32</v>
+        <v>7.98</v>
       </c>
       <c r="G9">
-        <v>108.28</v>
+        <v>15.41</v>
       </c>
       <c r="H9">
-        <v>161.85</v>
+        <v>23.49</v>
       </c>
       <c r="I9">
-        <v>76.989999999999995</v>
+        <v>14</v>
       </c>
       <c r="J9">
-        <v>544.73</v>
+        <v>67.55</v>
       </c>
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>11</v>
+        <v>53</v>
       </c>
       <c r="B10">
-        <v>27.24</v>
+        <v>10.48</v>
       </c>
       <c r="C10">
-        <v>44.76</v>
+        <v>17.95</v>
       </c>
       <c r="D10">
-        <v>28.72</v>
+        <v>7.17</v>
       </c>
       <c r="E10">
-        <v>106.2</v>
+        <v>32.81</v>
       </c>
       <c r="F10">
-        <v>114.36</v>
+        <v>36.81</v>
       </c>
       <c r="G10">
-        <v>325.10000000000002</v>
+        <v>75.44</v>
       </c>
       <c r="H10">
-        <v>97.44</v>
+        <v>135.86000000000001</v>
       </c>
       <c r="I10">
-        <v>65.52</v>
+        <v>62.03</v>
       </c>
       <c r="J10">
-        <v>227.27</v>
+        <v>460.46</v>
       </c>
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>70</v>
-      </c>
-      <c r="B11" s="4">
-        <f>B6/B5</f>
-        <v>0</v>
-      </c>
-      <c r="C11" s="4">
-        <f t="shared" ref="C11:J11" si="0">C6/C5</f>
-        <v>0</v>
-      </c>
-      <c r="D11" s="4">
-        <f t="shared" si="0"/>
-        <v>1E-3</v>
-      </c>
-      <c r="E11" s="4">
-        <f t="shared" si="0"/>
-        <v>4.0294117647058827E-2</v>
-      </c>
-      <c r="F11" s="4">
-        <f t="shared" si="0"/>
-        <v>4.7894736842105268E-2</v>
-      </c>
-      <c r="G11" s="4">
-        <f t="shared" si="0"/>
-        <v>0.14841121495327103</v>
-      </c>
-      <c r="H11" s="4">
-        <f t="shared" si="0"/>
-        <v>4.4411764705882352E-2</v>
-      </c>
-      <c r="I11" s="4">
-        <f t="shared" si="0"/>
-        <v>2.4090909090909093E-2</v>
-      </c>
-      <c r="J11" s="4">
-        <f t="shared" si="0"/>
-        <v>0.18782051282051282</v>
+        <v>63</v>
+      </c>
+      <c r="B11">
+        <v>10.97</v>
+      </c>
+      <c r="C11">
+        <v>18.87</v>
+      </c>
+      <c r="D11">
+        <v>8.4600000000000009</v>
+      </c>
+      <c r="E11">
+        <v>42.43</v>
+      </c>
+      <c r="F11">
+        <v>47.32</v>
+      </c>
+      <c r="G11">
+        <v>108.28</v>
+      </c>
+      <c r="H11">
+        <v>161.85</v>
+      </c>
+      <c r="I11">
+        <v>76.989999999999995</v>
+      </c>
+      <c r="J11">
+        <v>544.73</v>
       </c>
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>71</v>
-      </c>
-      <c r="B12" s="4">
-        <f>B7/B5</f>
-        <v>4.7142857142857146E-2</v>
-      </c>
-      <c r="C12" s="4">
-        <f t="shared" ref="C12:J12" si="1">C7/C5</f>
-        <v>5.909090909090909E-2</v>
-      </c>
-      <c r="D12" s="4">
-        <f t="shared" si="1"/>
-        <v>0.10600000000000001</v>
-      </c>
-      <c r="E12" s="4">
-        <f t="shared" si="1"/>
-        <v>0.22588235294117645</v>
-      </c>
-      <c r="F12" s="4">
-        <f t="shared" si="1"/>
-        <v>0.21000000000000002</v>
-      </c>
-      <c r="G12" s="4">
-        <f t="shared" si="1"/>
-        <v>0.14401869158878505</v>
-      </c>
-      <c r="H12" s="4">
-        <f t="shared" si="1"/>
-        <v>0.69088235294117639</v>
-      </c>
-      <c r="I12" s="4">
-        <f t="shared" si="1"/>
-        <v>0.63636363636363635</v>
-      </c>
-      <c r="J12" s="4">
-        <f t="shared" si="1"/>
-        <v>0.86602564102564095</v>
+        <v>11</v>
+      </c>
+      <c r="B12">
+        <v>27.24</v>
+      </c>
+      <c r="C12">
+        <v>44.76</v>
+      </c>
+      <c r="D12">
+        <v>28.72</v>
+      </c>
+      <c r="E12">
+        <v>106.2</v>
+      </c>
+      <c r="F12">
+        <v>114.36</v>
+      </c>
+      <c r="G12">
+        <v>325.10000000000002</v>
+      </c>
+      <c r="H12">
+        <v>97.44</v>
+      </c>
+      <c r="I12">
+        <v>65.52</v>
+      </c>
+      <c r="J12">
+        <v>227.27</v>
       </c>
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="B13" s="4">
-        <f>B8/B5</f>
-        <v>1.4971428571428571</v>
+        <f>B8/B7</f>
+        <v>0</v>
       </c>
       <c r="C13" s="4">
-        <f t="shared" ref="C13:J13" si="2">C8/C5</f>
-        <v>1.6318181818181818</v>
+        <f t="shared" ref="C13:J13" si="1">C8/C7</f>
+        <v>0</v>
       </c>
       <c r="D13" s="4">
-        <f t="shared" si="2"/>
-        <v>0.71699999999999997</v>
+        <f t="shared" si="1"/>
+        <v>1E-3</v>
       </c>
       <c r="E13" s="4">
-        <f t="shared" si="2"/>
-        <v>0.96500000000000008</v>
+        <f t="shared" si="1"/>
+        <v>4.0294117647058827E-2</v>
       </c>
       <c r="F13" s="4">
-        <f t="shared" si="2"/>
-        <v>0.96868421052631581</v>
+        <f t="shared" si="1"/>
+        <v>4.7894736842105268E-2</v>
       </c>
       <c r="G13" s="4">
-        <f t="shared" si="2"/>
-        <v>0.70504672897196263</v>
+        <f t="shared" si="1"/>
+        <v>0.14841121495327103</v>
       </c>
       <c r="H13" s="4">
-        <f t="shared" si="2"/>
-        <v>3.9958823529411767</v>
+        <f t="shared" si="1"/>
+        <v>4.4411764705882352E-2</v>
       </c>
       <c r="I13" s="4">
-        <f t="shared" si="2"/>
-        <v>2.8195454545454548</v>
+        <f t="shared" si="1"/>
+        <v>2.4090909090909093E-2</v>
       </c>
       <c r="J13" s="4">
-        <f t="shared" si="2"/>
-        <v>5.9033333333333333</v>
+        <f t="shared" si="1"/>
+        <v>0.18782051282051282</v>
       </c>
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="B14" s="4">
-        <f>B9/B5</f>
-        <v>1.5671428571428572</v>
+        <f>B9/B7</f>
+        <v>4.7142857142857146E-2</v>
       </c>
       <c r="C14" s="4">
-        <f t="shared" ref="C14:J14" si="3">C9/C5</f>
-        <v>1.7154545454545456</v>
+        <f t="shared" ref="C14:J14" si="2">C9/C7</f>
+        <v>5.909090909090909E-2</v>
       </c>
       <c r="D14" s="4">
-        <f t="shared" si="3"/>
-        <v>0.84600000000000009</v>
+        <f t="shared" si="2"/>
+        <v>0.10600000000000001</v>
       </c>
       <c r="E14" s="4">
-        <f t="shared" si="3"/>
-        <v>1.2479411764705883</v>
+        <f t="shared" si="2"/>
+        <v>0.22588235294117645</v>
       </c>
       <c r="F14" s="4">
-        <f t="shared" si="3"/>
-        <v>1.2452631578947368</v>
+        <f t="shared" si="2"/>
+        <v>0.21000000000000002</v>
       </c>
       <c r="G14" s="4">
-        <f t="shared" si="3"/>
-        <v>1.0119626168224298</v>
+        <f t="shared" si="2"/>
+        <v>0.14401869158878505</v>
       </c>
       <c r="H14" s="4">
-        <f t="shared" si="3"/>
-        <v>4.7602941176470583</v>
+        <f t="shared" si="2"/>
+        <v>0.69088235294117639</v>
       </c>
       <c r="I14" s="4">
-        <f t="shared" si="3"/>
-        <v>3.4995454545454545</v>
+        <f t="shared" si="2"/>
+        <v>0.63636363636363635</v>
       </c>
       <c r="J14" s="4">
-        <f t="shared" si="3"/>
-        <v>6.983717948717949</v>
+        <f t="shared" si="2"/>
+        <v>0.86602564102564095</v>
       </c>
     </row>
     <row r="15" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
+        <v>72</v>
+      </c>
+      <c r="B15" s="4">
+        <f>B10/B7</f>
+        <v>1.4971428571428571</v>
+      </c>
+      <c r="C15" s="4">
+        <f t="shared" ref="C15:J15" si="3">C10/C7</f>
+        <v>1.6318181818181818</v>
+      </c>
+      <c r="D15" s="4">
+        <f t="shared" si="3"/>
+        <v>0.71699999999999997</v>
+      </c>
+      <c r="E15" s="4">
+        <f t="shared" si="3"/>
+        <v>0.96500000000000008</v>
+      </c>
+      <c r="F15" s="4">
+        <f t="shared" si="3"/>
+        <v>0.96868421052631581</v>
+      </c>
+      <c r="G15" s="4">
+        <f t="shared" si="3"/>
+        <v>0.70504672897196263</v>
+      </c>
+      <c r="H15" s="4">
+        <f t="shared" si="3"/>
+        <v>3.9958823529411767</v>
+      </c>
+      <c r="I15" s="4">
+        <f t="shared" si="3"/>
+        <v>2.8195454545454548</v>
+      </c>
+      <c r="J15" s="4">
+        <f t="shared" si="3"/>
+        <v>5.9033333333333333</v>
+      </c>
+    </row>
+    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>73</v>
+      </c>
+      <c r="B16" s="4">
+        <f>B11/B7</f>
+        <v>1.5671428571428572</v>
+      </c>
+      <c r="C16" s="4">
+        <f t="shared" ref="C16:J16" si="4">C11/C7</f>
+        <v>1.7154545454545456</v>
+      </c>
+      <c r="D16" s="4">
+        <f t="shared" si="4"/>
+        <v>0.84600000000000009</v>
+      </c>
+      <c r="E16" s="4">
+        <f t="shared" si="4"/>
+        <v>1.2479411764705883</v>
+      </c>
+      <c r="F16" s="4">
+        <f t="shared" si="4"/>
+        <v>1.2452631578947368</v>
+      </c>
+      <c r="G16" s="4">
+        <f t="shared" si="4"/>
+        <v>1.0119626168224298</v>
+      </c>
+      <c r="H16" s="4">
+        <f t="shared" si="4"/>
+        <v>4.7602941176470583</v>
+      </c>
+      <c r="I16" s="4">
+        <f t="shared" si="4"/>
+        <v>3.4995454545454545</v>
+      </c>
+      <c r="J16" s="4">
+        <f t="shared" si="4"/>
+        <v>6.983717948717949</v>
+      </c>
+    </row>
+    <row r="17" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
         <v>74</v>
       </c>
-      <c r="B15" s="4">
-        <f>B4/B5</f>
+      <c r="B17" s="4">
+        <f>B6/B7</f>
         <v>12.571428571428571</v>
       </c>
-      <c r="C15" s="4">
-        <f t="shared" ref="C15:J15" si="4">C4/C5</f>
+      <c r="C17" s="4">
+        <f t="shared" ref="C17:J17" si="5">C6/C7</f>
         <v>13.272727272727273</v>
       </c>
-      <c r="D15" s="4">
-        <f t="shared" si="4"/>
+      <c r="D17" s="4">
+        <f t="shared" si="5"/>
         <v>9.6</v>
       </c>
-      <c r="E15" s="4">
-        <f t="shared" si="4"/>
+      <c r="E17" s="4">
+        <f t="shared" si="5"/>
         <v>40.941176470588232</v>
       </c>
-      <c r="F15" s="4">
-        <f t="shared" si="4"/>
+      <c r="F17" s="4">
+        <f t="shared" si="5"/>
         <v>39.210526315789473</v>
       </c>
-      <c r="G15" s="4">
-        <f t="shared" si="4"/>
+      <c r="G17" s="4">
+        <f t="shared" si="5"/>
         <v>40.420560747663551</v>
       </c>
-      <c r="H15" s="4">
-        <f t="shared" si="4"/>
+      <c r="H17" s="4">
+        <f t="shared" si="5"/>
         <v>38.588235294117645</v>
       </c>
-      <c r="I15" s="4">
-        <f t="shared" si="4"/>
+      <c r="I17" s="4">
+        <f t="shared" si="5"/>
         <v>39.272727272727273</v>
       </c>
-      <c r="J15" s="4">
-        <f t="shared" si="4"/>
+      <c r="J17" s="4">
+        <f t="shared" si="5"/>
         <v>38.987179487179489</v>
       </c>
     </row>
@@ -30092,8 +30210,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:P9"/>
   <sheetViews>
-    <sheetView topLeftCell="A9" workbookViewId="0">
-      <selection activeCell="B1" sqref="B1"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="P4" sqref="P4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -30390,8 +30508,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:P9"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B1" sqref="B1"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="S9" sqref="S9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -30409,31 +30527,31 @@
     </row>
     <row r="2" spans="1:16" x14ac:dyDescent="0.25">
       <c r="B2">
-        <v>6</v>
+        <v>20</v>
       </c>
       <c r="C2">
-        <v>12</v>
+        <v>40</v>
       </c>
       <c r="D2">
-        <v>24</v>
+        <v>80</v>
       </c>
       <c r="H2">
-        <v>6</v>
+        <v>20</v>
       </c>
       <c r="I2">
-        <v>12</v>
+        <v>40</v>
       </c>
       <c r="J2">
-        <v>24</v>
+        <v>80</v>
       </c>
       <c r="N2">
-        <v>6</v>
+        <v>20</v>
       </c>
       <c r="O2">
-        <v>12</v>
+        <v>40</v>
       </c>
       <c r="P2">
-        <v>24</v>
+        <v>80</v>
       </c>
     </row>
     <row r="3" spans="1:16" x14ac:dyDescent="0.25">
@@ -30759,10 +30877,10 @@
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K9"/>
+  <dimension ref="A1:K11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="O5" sqref="O5"/>
+      <selection activeCell="J10" sqref="J10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -30972,6 +31090,64 @@
       <c r="K9">
         <f t="shared" ref="K9" si="3">1.96*K6/SQRT(K7)</f>
         <v>0.92661059998253847</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>77</v>
+      </c>
+      <c r="B10">
+        <f>B4/B3</f>
+        <v>0.13172645739910316</v>
+      </c>
+      <c r="C10">
+        <f t="shared" ref="C10:K10" si="4">C4/C3</f>
+        <v>0.37667698658410731</v>
+      </c>
+      <c r="F10">
+        <f t="shared" si="4"/>
+        <v>0.10194174757281553</v>
+      </c>
+      <c r="G10">
+        <f t="shared" si="4"/>
+        <v>0.19806206021455763</v>
+      </c>
+      <c r="J10">
+        <f t="shared" si="4"/>
+        <v>0.14697383207577461</v>
+      </c>
+      <c r="K10">
+        <f t="shared" si="4"/>
+        <v>0.17841462250644269</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>78</v>
+      </c>
+      <c r="B11">
+        <f>B6/B5</f>
+        <v>6.720430107526881E-3</v>
+      </c>
+      <c r="C11">
+        <f t="shared" ref="C11:K11" si="5">C6/C5</f>
+        <v>3.9197602029052347E-3</v>
+      </c>
+      <c r="F11">
+        <f t="shared" si="5"/>
+        <v>1.655535697488477E-2</v>
+      </c>
+      <c r="G11">
+        <f t="shared" si="5"/>
+        <v>6.8834796488427769E-3</v>
+      </c>
+      <c r="J11">
+        <f t="shared" si="5"/>
+        <v>9.0035407182599905E-3</v>
+      </c>
+      <c r="K11">
+        <f t="shared" si="5"/>
+        <v>3.240489866695568E-2</v>
       </c>
     </row>
   </sheetData>
@@ -30984,7 +31160,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:P9"/>
   <sheetViews>
-    <sheetView topLeftCell="A9" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>

</xml_diff>